<commit_message>
added item-based collaborative filtering notebook
</commit_message>
<xml_diff>
--- a/Chapter 29 - Netflix Recommendations/FinalItemBased.xlsx
+++ b/Chapter 29 - Netflix Recommendations/FinalItemBased.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\wiley29\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/walter/Desktop/SCRATCH_CODE/analytics-stories/Chapter 29 - Netflix Recommendations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F2A8B4-B26E-47D4-9942-39380791DCA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C7F304-7F18-B64B-B5DC-994BD5A6FBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53540" yWindow="2420" windowWidth="36240" windowHeight="23420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Correlation sim" sheetId="4" r:id="rId1"/>
@@ -518,33 +518,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B7:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.09765625" style="1"/>
-    <col min="3" max="3" width="20.8984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.296875" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="20.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="6" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.3984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.3984375" style="1" customWidth="1"/>
-    <col min="11" max="13" width="9.09765625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.09765625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.09765625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.3984375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.69921875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="9.09765625" style="1"/>
-    <col min="20" max="20" width="11.3984375" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.09765625" style="1"/>
+    <col min="6" max="6" width="9.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" style="1" customWidth="1"/>
+    <col min="11" max="13" width="9.1640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="9.1640625" style="1"/>
+    <col min="20" max="20" width="11.33203125" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.2">
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
@@ -567,7 +567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
@@ -591,7 +591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
@@ -618,7 +618,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
@@ -639,7 +639,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
@@ -663,7 +663,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
@@ -690,7 +690,7 @@
         <v>2.8333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>6</v>
       </c>
@@ -714,7 +714,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
@@ -732,7 +732,7 @@
         <v>3.1666666666666665</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.2">
       <c r="D15" s="1">
         <v>1</v>
       </c>
@@ -752,7 +752,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
         <v>20</v>
       </c>
@@ -781,7 +781,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
         <v>23</v>
       </c>
@@ -810,7 +810,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="str">
         <f>C16</f>
         <v>Still Alice</v>
@@ -843,7 +843,7 @@
       <c r="P18" s="2"/>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="str">
         <f>C17</f>
         <v>DodgeBall</v>
@@ -876,7 +876,7 @@
       <c r="P19" s="2"/>
       <c r="R19" s="2"/>
     </row>
-    <row r="21" spans="2:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" ht="48" x14ac:dyDescent="0.2">
       <c r="D21" s="3" t="s">
         <v>10</v>
       </c>
@@ -903,7 +903,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D22" s="4">
         <f>CORREL(D18:I18,D19:I19)</f>
         <v>-0.48566186425718266</v>
@@ -931,7 +931,7 @@
         <v>-1.0000000000000002</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.2">
       <c r="N23" s="1" t="s">
         <v>22</v>
       </c>
@@ -954,7 +954,7 @@
         <v>-0.63386569104638746</v>
       </c>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.2">
       <c r="N24" s="1" t="s">
         <v>20</v>
       </c>
@@ -977,7 +977,7 @@
         <v>0.94491118252306805</v>
       </c>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D25" s="1" t="s">
         <v>15</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>-0.29646353064078551</v>
       </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>11</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>-0.33333333333333331</v>
       </c>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>12</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.2">
       <c r="E28" s="1" t="s">
         <v>13</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C29" s="1">
         <v>1</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C30" s="1">
         <v>2</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C31" s="1">
         <v>3</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C32" s="1">
         <v>4</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>0.42289003161103106</v>
       </c>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C33" s="1">
         <v>5</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>0.48566186425718266</v>
       </c>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C34" s="1">
         <v>6</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
         <v>17</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>=SUMPRODUCT(G29:G34,F29:F34)/SUM(H29:H34)</v>
       </c>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
         <v>18</v>
       </c>
@@ -1266,6 +1266,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010024A92190D758C14CABA06EB5DDDCFAB6" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d4d4151efdceb84e9b5f2f7e6aee3da">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9bdcab5d-de70-4d4a-a9b3-2de08f1afc7f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="23ee0c930fb979ef27d10e53ad7fa985" ns2:_="">
     <xsd:import namespace="9bdcab5d-de70-4d4a-a9b3-2de08f1afc7f"/>
@@ -1443,29 +1458,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ED7DDCA-68FF-4EEC-9BCB-5055D3AFF0F8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C7BA3F8-19E6-4ED7-9E7F-48A38E00237B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8017F0E3-3E63-4212-AF6D-1137B9FE1263}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8017F0E3-3E63-4212-AF6D-1137B9FE1263}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C7BA3F8-19E6-4ED7-9E7F-48A38E00237B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ED7DDCA-68FF-4EEC-9BCB-5055D3AFF0F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9bdcab5d-de70-4d4a-a9b3-2de08f1afc7f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>